<commit_message>
Actualizacion Escenarios Pruebas exploratorias
</commit_message>
<xml_diff>
--- a/Videos/inventario-pruebas-exploratorias.xlsx
+++ b/Videos/inventario-pruebas-exploratorias.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\PruebasAutomatizadas\Videos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Andes\Ciclo2\Pruebas\RepoKarenMay21\PruebasAutomatizadas\Videos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA170D5-654C-44D8-8ADF-8F6E2EDC1371}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FD708C-AFC6-434B-90B8-E46794E4C18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="108">
   <si>
     <t>Funcionalidad</t>
   </si>
@@ -345,6 +345,18 @@
   </si>
   <si>
     <t>Crear una pagina borrador</t>
+  </si>
+  <si>
+    <t>No se deberia poder crear un Post sin Titulos.</t>
+  </si>
+  <si>
+    <t>No se deberia poder crear un Post sin detalles.</t>
+  </si>
+  <si>
+    <t>Deja crear Post sin titulos ni detalle</t>
+  </si>
+  <si>
+    <t>Deja ingresar solo caracteres especiales.</t>
   </si>
 </sst>
 </file>
@@ -512,9 +524,63 @@
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -523,60 +589,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -916,926 +928,934 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="F7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="21.625" style="15"/>
-    <col min="3" max="3" width="14.875" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.25" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="75.375" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.25" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="63.625" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.875" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37.125" style="9" customWidth="1"/>
-    <col min="11" max="16384" width="21.625" style="15"/>
+    <col min="1" max="1" width="21.625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="21.625" style="8"/>
+    <col min="3" max="3" width="14.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.25" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.25" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="63.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="21.625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-    </row>
-    <row r="2" spans="2:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="2:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="2:10" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+    </row>
+    <row r="3" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="2:10" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="2:10" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="22"/>
+    </row>
+    <row r="5" spans="2:10" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="2:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="22"/>
+    </row>
+    <row r="6" spans="2:10" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="2:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-    </row>
-    <row r="8" spans="2:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="19"/>
+    </row>
+    <row r="7" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="2:10" s="9" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+    </row>
+    <row r="9" spans="2:10" s="2" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="J9" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="13">
+    <row r="10" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
         <v>1</v>
       </c>
-      <c r="C10" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D10" s="17" t="s">
+      <c r="C10" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="21" t="s">
+      <c r="F10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="J10" s="14"/>
+      <c r="J10" s="7" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="13">
+      <c r="B11" s="6">
         <v>2</v>
       </c>
-      <c r="C11" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D11" s="17" t="s">
+      <c r="C11" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="21" t="s">
+      <c r="F11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="J11" s="14"/>
+      <c r="J11" s="7"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="13">
+      <c r="B12" s="6">
         <v>3</v>
       </c>
-      <c r="C12" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D12" s="17" t="s">
+      <c r="C12" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="21" t="s">
+      <c r="F12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="J12" s="14"/>
+      <c r="J12" s="7"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="13">
+      <c r="B13" s="6">
         <v>4</v>
       </c>
-      <c r="C13" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D13" s="17" t="s">
+      <c r="C13" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F13" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="21" t="s">
+      <c r="F13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="I13" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="J13" s="14"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="13">
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
         <v>5</v>
       </c>
-      <c r="C14" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D14" s="17" t="s">
+      <c r="C14" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="F14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="21" t="s">
+      <c r="F14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="I14" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="J14" s="14"/>
+      <c r="J14" s="7" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="13">
+      <c r="B15" s="6">
         <v>6</v>
       </c>
-      <c r="C15" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D15" s="17" t="s">
+      <c r="C15" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F15" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="21" t="s">
+      <c r="F15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="J15" s="14"/>
+      <c r="J15" s="7"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="13">
+      <c r="B16" s="6">
         <v>7</v>
       </c>
-      <c r="C16" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D16" s="17" t="s">
+      <c r="C16" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F16" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="21" t="s">
+      <c r="F16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="I16" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J16" s="14"/>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="13">
+      <c r="B17" s="6">
         <v>8</v>
       </c>
-      <c r="C17" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D17" s="17" t="s">
+      <c r="C17" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="F17" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="21" t="s">
+      <c r="F17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="I17" s="17" t="s">
+      <c r="I17" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="J17" s="14"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="13">
+      <c r="J17" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="6">
         <v>9</v>
       </c>
-      <c r="C18" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D18" s="17" t="s">
+      <c r="C18" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F18" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="21" t="s">
+      <c r="F18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="I18" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="J18" s="14"/>
+      <c r="J18" s="7" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="13">
+      <c r="B19" s="6">
         <v>10</v>
       </c>
-      <c r="C19" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D19" s="17" t="s">
+      <c r="C19" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F19" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="21" t="s">
+      <c r="F19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="I19" s="17" t="s">
+      <c r="I19" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="J19" s="14"/>
+      <c r="J19" s="7"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="13">
+      <c r="B20" s="6">
         <v>11</v>
       </c>
-      <c r="C20" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D20" s="17" t="s">
+      <c r="C20" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E20" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="F20" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="21" t="s">
+      <c r="F20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J20" s="14"/>
+      <c r="J20" s="7"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="13">
-        <v>12</v>
-      </c>
-      <c r="C21" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D21" s="17" t="s">
+      <c r="B21" s="6">
+        <v>12</v>
+      </c>
+      <c r="C21" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="E21" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="21" t="s">
+      <c r="F21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I21" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="J21" s="14"/>
+      <c r="J21" s="7"/>
     </row>
     <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="13">
+      <c r="B22" s="6">
         <v>13</v>
       </c>
-      <c r="C22" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D22" s="13" t="s">
+      <c r="C22" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="E22" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="21" t="s">
+      <c r="F22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="I22" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="J22" s="18" t="s">
+      <c r="J22" s="11" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="13">
-        <v>14</v>
-      </c>
-      <c r="C23" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D23" s="13" t="s">
+      <c r="B23" s="6">
+        <v>14</v>
+      </c>
+      <c r="C23" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="E23" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23" s="21" t="s">
+      <c r="F23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="I23" s="17" t="s">
+      <c r="I23" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="J23" s="14"/>
+      <c r="J23" s="7"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="13">
+      <c r="B24" s="6">
         <v>15</v>
       </c>
-      <c r="C24" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D24" s="13" t="s">
+      <c r="C24" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="21" t="s">
+      <c r="E24" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24" s="21" t="s">
+      <c r="F24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I24" s="17" t="s">
+      <c r="I24" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J24" s="14"/>
+      <c r="J24" s="7"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="13">
+      <c r="B25" s="6">
         <v>16</v>
       </c>
-      <c r="C25" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D25" s="13" t="s">
+      <c r="C25" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="21" t="s">
+      <c r="F25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="I25" s="17" t="s">
+      <c r="I25" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="J25" s="14"/>
+      <c r="J25" s="7"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="13">
+      <c r="B26" s="6">
         <v>17</v>
       </c>
-      <c r="C26" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D26" s="13" t="s">
+      <c r="C26" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="21" t="s">
+      <c r="F26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="I26" s="17" t="s">
+      <c r="I26" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="J26" s="14"/>
+      <c r="J26" s="7"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="13">
+      <c r="B27" s="6">
         <v>18</v>
       </c>
-      <c r="C27" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D27" s="13" t="s">
+      <c r="C27" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="21" t="s">
+      <c r="F27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="I27" s="17" t="s">
+      <c r="I27" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="J27" s="14"/>
+      <c r="J27" s="7"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="13">
+      <c r="B28" s="6">
         <v>19</v>
       </c>
-      <c r="C28" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D28" s="13" t="s">
+      <c r="C28" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F28" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="21" t="s">
+      <c r="F28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I28" s="17" t="s">
+      <c r="I28" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="J28" s="14"/>
+      <c r="J28" s="7"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="13">
+      <c r="B29" s="6">
         <v>20</v>
       </c>
-      <c r="C29" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D29" s="13" t="s">
+      <c r="C29" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E29" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F29" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" s="21" t="s">
+      <c r="F29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I29" s="17" t="s">
+      <c r="I29" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J29" s="14"/>
+      <c r="J29" s="7"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="13">
+      <c r="B30" s="6">
         <v>21</v>
       </c>
-      <c r="C30" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D30" s="13" t="s">
+      <c r="C30" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H30" s="21" t="s">
+      <c r="F30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="I30" s="17" t="s">
+      <c r="I30" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="J30" s="14"/>
+      <c r="J30" s="7"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="13">
+      <c r="B31" s="6">
         <v>22</v>
       </c>
-      <c r="C31" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D31" s="13" t="s">
+      <c r="C31" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F31" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31" s="21" t="s">
+      <c r="F31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="I31" s="17" t="s">
+      <c r="I31" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="J31" s="14"/>
+      <c r="J31" s="7"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="13">
+      <c r="B32" s="6">
         <v>23</v>
       </c>
-      <c r="C32" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D32" s="13" t="s">
+      <c r="C32" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="E32" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F32" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H32" s="21" t="s">
+      <c r="F32" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="I32" s="17" t="s">
+      <c r="I32" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="J32" s="14"/>
+      <c r="J32" s="7"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="13">
+      <c r="B33" s="6">
         <v>24</v>
       </c>
-      <c r="C33" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D33" s="13" t="s">
+      <c r="C33" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E33" s="22" t="s">
+      <c r="E33" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="F33" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33" s="21" t="s">
+      <c r="F33" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="I33" s="17" t="s">
+      <c r="I33" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="J33" s="14"/>
+      <c r="J33" s="7"/>
     </row>
     <row r="34" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B34" s="13">
+      <c r="B34" s="6">
         <v>25</v>
       </c>
-      <c r="C34" s="16">
-        <v>44343</v>
-      </c>
-      <c r="D34" s="13" t="s">
+      <c r="C34" s="9">
+        <v>44343</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E34" s="21" t="s">
+      <c r="E34" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F34" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34" s="21" t="s">
+      <c r="F34" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="I34" s="17" t="s">
+      <c r="I34" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="J34" s="18" t="s">
+      <c r="J34" s="11" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="8"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="1"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="8"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="1"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="8"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="1"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="8"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="1"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="8"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="1"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="8"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="1"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="8"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="1"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>